<commit_message>
arranged some program around person data system
</commit_message>
<xml_diff>
--- a/components/importFile/インポートフォーマット（記入例）.xlsx
+++ b/components/importFile/インポートフォーマット（記入例）.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>整理番号</t>
     <rPh sb="0" eb="2">
@@ -124,6 +124,13 @@
   </si>
   <si>
     <t>坂牛 隆樹</t>
+  </si>
+  <si>
+    <t>備考</t>
+    <rPh sb="0" eb="2">
+      <t>ビコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -195,15 +202,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>649941</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>123265</xdr:rowOff>
+      <xdr:colOff>78441</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>22413</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>638736</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>78442</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>280148</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>168089</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -218,13 +225,13 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2756647" y="123265"/>
-          <a:ext cx="2723030" cy="896471"/>
+          <a:off x="2185147" y="493060"/>
+          <a:ext cx="2252383" cy="1322294"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -79268"/>
-            <a:gd name="adj2" fmla="val -48931"/>
+            <a:gd name="adj1" fmla="val -67021"/>
+            <a:gd name="adj2" fmla="val -63889"/>
             <a:gd name="adj3" fmla="val 16667"/>
           </a:avLst>
         </a:prstGeom>
@@ -260,14 +267,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>6723</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>421341</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>129989</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>679077</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>410135</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>179294</xdr:rowOff>
     </xdr:to>
@@ -284,13 +291,13 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2796988" y="1071283"/>
+          <a:off x="4578723" y="1071283"/>
           <a:ext cx="2723030" cy="1696570"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -84207"/>
-            <a:gd name="adj2" fmla="val 5635"/>
+            <a:gd name="adj1" fmla="val -149639"/>
+            <a:gd name="adj2" fmla="val 4314"/>
             <a:gd name="adj3" fmla="val 16667"/>
           </a:avLst>
         </a:prstGeom>
@@ -342,16 +349,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>47064</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>35859</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>439270</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>226358</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>35859</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>428064</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>100852</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -366,13 +373,13 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2837329" y="2859741"/>
-          <a:ext cx="2723030" cy="1846730"/>
+          <a:off x="4596652" y="2814917"/>
+          <a:ext cx="2723030" cy="1992406"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRoundRectCallout">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -96140"/>
-            <a:gd name="adj2" fmla="val 32594"/>
+            <a:gd name="adj1" fmla="val -157456"/>
+            <a:gd name="adj2" fmla="val 28657"/>
             <a:gd name="adj3" fmla="val 16667"/>
           </a:avLst>
         </a:prstGeom>
@@ -439,6 +446,72 @@
           <a:r>
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
             <a:t>は第二部の整理番号として機能を追加します（範囲は後から設定で変更可能）</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>510989</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>51547</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>235324</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>6724</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="吹き出し: 角を丸めた四角形 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0222703-0E38-41FC-88F4-370691B5994F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4668371" y="51547"/>
+          <a:ext cx="1775012" cy="896471"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -158369"/>
+            <a:gd name="adj2" fmla="val -37681"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>備考の列には、アプリでも見れるコメントを記述できます。</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
         </a:p>
@@ -746,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -757,15 +830,18 @@
     <col min="2" max="2" width="18.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -773,7 +849,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -781,7 +857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -789,7 +865,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>4</v>
       </c>
@@ -797,7 +873,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -805,7 +881,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>6</v>
       </c>
@@ -813,7 +889,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>7</v>
       </c>
@@ -821,7 +897,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>8</v>
       </c>
@@ -829,7 +905,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>9</v>
       </c>
@@ -837,7 +913,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>10</v>
       </c>
@@ -845,7 +921,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>11</v>
       </c>
@@ -853,7 +929,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>12</v>
       </c>
@@ -861,7 +937,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>13</v>
       </c>
@@ -869,7 +945,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -877,7 +953,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>250</v>
       </c>

</xml_diff>